<commit_message>
figure updates and rerunning Pathfinder GLS function
</commit_message>
<xml_diff>
--- a/data/Supplemental_Tables.xlsx
+++ b/data/Supplemental_Tables.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -15,46 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
-  <si>
-    <t xml:space="preserve">Temperature.parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HadISST..1871.2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HadISST..1981.2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HadISST..1987.2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathfinder..1981.2019.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathfinder..1990.2019.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caribbean Basin (°C per decade)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caribbean Basin (total °C for period)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caribbean Reefs (°C per decade)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caribbean Reefs (total °C for period)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.66</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">ecoregion</t>
   </si>
@@ -161,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -480,132 +441,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="38.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="19.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="19.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="19.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="22.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="22.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="9.15" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="9.15" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="9.15" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="9.15" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="9.15" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="9.15" hidden="0" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -619,27 +479,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
         <v>1988</v>
@@ -659,7 +519,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
         <v>1984</v>
@@ -679,7 +539,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
         <v>1993</v>
@@ -699,7 +559,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
         <v>1986</v>
@@ -719,7 +579,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B6" t="n">
         <v>1981</v>
@@ -739,7 +599,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B7" t="n">
         <v>1981</v>
@@ -759,7 +619,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B8" t="n">
         <v>1982</v>
@@ -779,7 +639,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
         <v>1999</v>
@@ -804,10 +664,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -820,24 +680,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B2" t="n">
         <v>-93.154</v>
@@ -849,12 +709,12 @@
         <v>-104.406</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B3" t="n">
         <v>0.047</v>
@@ -866,12 +726,12 @@
         <v>105.559</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B4" t="n">
         <v>0.48</v>
@@ -879,12 +739,12 @@
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B5" t="n">
         <v>-36.508</v>
@@ -896,12 +756,12 @@
         <v>-54.79</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B6" t="n">
         <v>0.019</v>
@@ -913,12 +773,12 @@
         <v>58.157</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B7" t="n">
         <v>0.185</v>
@@ -926,12 +786,12 @@
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
         <v>87.968</v>
@@ -943,12 +803,12 @@
         <v>52.75</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
         <v>-0.041</v>
@@ -960,12 +820,12 @@
         <v>-49.84</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B10" t="n">
         <v>0.148</v>
@@ -973,7 +833,7 @@
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -983,10 +843,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -999,30 +859,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C2" t="n">
         <v>7.6</v>
@@ -1039,10 +899,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>8.6</v>
@@ -1059,10 +919,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
         <v>6.9</v>
@@ -1079,10 +939,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
         <v>8.9</v>
@@ -1099,10 +959,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
         <v>7.3</v>
@@ -1119,10 +979,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
         <v>8.2</v>
@@ -1139,10 +999,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C8" t="n">
         <v>7.5</v>
@@ -1159,10 +1019,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>7.3</v>
@@ -1179,10 +1039,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
         <v>7.1</v>
@@ -1199,10 +1059,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C11" t="n">
         <v>1.2</v>
@@ -1219,10 +1079,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
         <v>1.6</v>
@@ -1239,10 +1099,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
         <v>0.5</v>
@@ -1259,10 +1119,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
         <v>1.2</v>
@@ -1279,10 +1139,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C15" t="n">
         <v>1.2</v>
@@ -1299,10 +1159,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C16" t="n">
         <v>1.5</v>
@@ -1319,10 +1179,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -1339,10 +1199,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
         <v>1.2</v>
@@ -1359,10 +1219,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C19" t="n">
         <v>1.6</v>
@@ -1379,10 +1239,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C20" t="n">
         <v>376.7</v>
@@ -1399,10 +1259,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
         <v>304.6</v>
@@ -1419,10 +1279,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C22" t="n">
         <v>721.9</v>
@@ -1439,10 +1299,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C23" t="n">
         <v>334.2</v>
@@ -1459,10 +1319,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C24" t="n">
         <v>398.9</v>
@@ -1479,10 +1339,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C25" t="n">
         <v>364.9</v>
@@ -1499,10 +1359,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C26" t="n">
         <v>327.8</v>
@@ -1519,10 +1379,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C27" t="n">
         <v>449.2</v>
@@ -1539,10 +1399,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C28" t="n">
         <v>299.3</v>

</xml_diff>

<commit_message>
updated figures with the new autocorrelation consideration and GAMMM
</commit_message>
<xml_diff>
--- a/data/Supplemental_Tables.xlsx
+++ b/data/Supplemental_Tables.xlsx
@@ -15,7 +15,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+  <si>
+    <t xml:space="preserve">Temperature.parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HadISST..1871.2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HadISST..1981.2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HadISST..1987.2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathfinder..1981.2019.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathfinder..1990.2019.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caribbean Basin (°C per decade)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caribbean Basin (total °C for period)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caribbean Reefs (°C per decade)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caribbean Reefs (total °C for period)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.66</t>
+  </si>
   <si>
     <t xml:space="preserve">ecoregion</t>
   </si>
@@ -448,14 +487,115 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="9.15" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="9.15" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="9.15" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="9.15" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="9.15" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="9.15" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="38.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="19.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="19.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="19.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="22.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="22.71" hidden="0" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -479,27 +619,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B2" t="n">
         <v>1988</v>
@@ -519,7 +659,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B3" t="n">
         <v>1984</v>
@@ -539,7 +679,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
         <v>1993</v>
@@ -559,7 +699,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B5" t="n">
         <v>1986</v>
@@ -579,7 +719,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B6" t="n">
         <v>1981</v>
@@ -599,7 +739,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B7" t="n">
         <v>1981</v>
@@ -619,7 +759,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B8" t="n">
         <v>1982</v>
@@ -639,7 +779,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B9" t="n">
         <v>1999</v>
@@ -680,24 +820,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B2" t="n">
         <v>-93.154</v>
@@ -709,12 +849,12 @@
         <v>-104.406</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
         <v>0.047</v>
@@ -726,12 +866,12 @@
         <v>105.559</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B4" t="n">
         <v>0.48</v>
@@ -739,12 +879,12 @@
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
         <v>-36.508</v>
@@ -756,12 +896,12 @@
         <v>-54.79</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
         <v>0.019</v>
@@ -773,12 +913,12 @@
         <v>58.157</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B7" t="n">
         <v>0.185</v>
@@ -786,12 +926,12 @@
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B8" t="n">
         <v>87.968</v>
@@ -803,12 +943,12 @@
         <v>52.75</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B9" t="n">
         <v>-0.041</v>
@@ -820,12 +960,12 @@
         <v>-49.84</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B10" t="n">
         <v>0.148</v>
@@ -833,7 +973,7 @@
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -859,30 +999,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C2" t="n">
         <v>7.6</v>
@@ -899,10 +1039,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C3" t="n">
         <v>8.6</v>
@@ -919,10 +1059,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
         <v>6.9</v>
@@ -939,10 +1079,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
         <v>8.9</v>
@@ -959,10 +1099,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C6" t="n">
         <v>7.3</v>
@@ -979,10 +1119,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C7" t="n">
         <v>8.2</v>
@@ -999,10 +1139,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C8" t="n">
         <v>7.5</v>
@@ -1019,10 +1159,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
         <v>7.3</v>
@@ -1039,10 +1179,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C10" t="n">
         <v>7.1</v>
@@ -1059,10 +1199,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C11" t="n">
         <v>1.2</v>
@@ -1079,10 +1219,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C12" t="n">
         <v>1.6</v>
@@ -1099,10 +1239,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C13" t="n">
         <v>0.5</v>
@@ -1119,10 +1259,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14" t="n">
         <v>1.2</v>
@@ -1139,10 +1279,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C15" t="n">
         <v>1.2</v>
@@ -1159,10 +1299,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C16" t="n">
         <v>1.5</v>
@@ -1179,10 +1319,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -1199,10 +1339,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C18" t="n">
         <v>1.2</v>
@@ -1219,10 +1359,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C19" t="n">
         <v>1.6</v>
@@ -1239,10 +1379,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C20" t="n">
         <v>376.7</v>
@@ -1259,10 +1399,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C21" t="n">
         <v>304.6</v>
@@ -1279,10 +1419,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C22" t="n">
         <v>721.9</v>
@@ -1299,10 +1439,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C23" t="n">
         <v>334.2</v>
@@ -1319,10 +1459,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C24" t="n">
         <v>398.9</v>
@@ -1339,10 +1479,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C25" t="n">
         <v>364.9</v>
@@ -1359,10 +1499,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C26" t="n">
         <v>327.8</v>
@@ -1379,10 +1519,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C27" t="n">
         <v>449.2</v>
@@ -1399,10 +1539,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C28" t="n">
         <v>299.3</v>

</xml_diff>

<commit_message>
added climate stripes figure and updates to figures
</commit_message>
<xml_diff>
--- a/data/Supplemental_Tables.xlsx
+++ b/data/Supplemental_Tables.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">HadISST..1981.2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">HadISST..1987.2020.</t>
+    <t xml:space="preserve">HadISST..1994.2020.</t>
   </si>
   <si>
     <t xml:space="preserve">Pathfinder..1981.2019.</t>
@@ -47,13 +47,13 @@
     <t xml:space="preserve">Caribbean Reefs (°C per decade)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.2</t>
+    <t xml:space="preserve">0.18</t>
   </si>
   <si>
     <t xml:space="preserve">Caribbean Reefs (total °C for period)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.66</t>
+    <t xml:space="preserve">0.47</t>
   </si>
   <si>
     <t xml:space="preserve">ecoregion</t>
@@ -526,7 +526,7 @@
         <v>0.17</v>
       </c>
       <c r="D2" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="E2" t="n">
         <v>0.17</v>
@@ -546,7 +546,7 @@
         <v>0.68</v>
       </c>
       <c r="D3" t="n">
-        <v>0.61</v>
+        <v>0.54</v>
       </c>
       <c r="E3" t="n">
         <v>0.66</v>
@@ -566,7 +566,7 @@
         <v>0.15</v>
       </c>
       <c r="D4" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="E4" t="n">
         <v>0.19</v>
@@ -586,7 +586,7 @@
         <v>0.6</v>
       </c>
       <c r="D5" t="n">
-        <v>0.54</v>
+        <v>0.46</v>
       </c>
       <c r="E5" t="n">
         <v>0.74</v>

</xml_diff>

<commit_message>
updated markdown based on manuscript resubmission
</commit_message>
<xml_diff>
--- a/data/Supplemental_Tables.xlsx
+++ b/data/Supplemental_Tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">Temperature.parameter</t>
   </si>
@@ -35,25 +35,67 @@
     <t xml:space="preserve">Pathfinder..1990.2019.</t>
   </si>
   <si>
+    <t xml:space="preserve">OISST</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caribbean Basin (°C per decade)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
     <t xml:space="preserve">Caribbean Basin (total °C for period)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.66</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caribbean Reefs (°C per decade)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.19</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.18</t>
   </si>
   <si>
     <t xml:space="preserve">Caribbean Reefs (total °C for period)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.74</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caribbean Basin (increasing frequency of MHW per year) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05</t>
   </si>
   <si>
     <t xml:space="preserve">ecoregion</t>
@@ -487,7 +529,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="38.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="55.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="19.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="19.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="19.71" hidden="0" customWidth="1"/>
@@ -514,85 +556,123 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.17</v>
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.66</v>
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.19</v>
+      <c r="E4" t="s">
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -619,27 +699,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B2" t="n">
         <v>1988</v>
@@ -659,7 +739,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
         <v>1984</v>
@@ -679,7 +759,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B4" t="n">
         <v>1993</v>
@@ -699,7 +779,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B5" t="n">
         <v>1986</v>
@@ -719,7 +799,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B6" t="n">
         <v>1981</v>
@@ -739,7 +819,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B7" t="n">
         <v>1981</v>
@@ -759,7 +839,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B8" t="n">
         <v>1982</v>
@@ -779,7 +859,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B9" t="n">
         <v>1999</v>
@@ -820,24 +900,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B2" t="n">
         <v>-93.154</v>
@@ -849,12 +929,12 @@
         <v>-104.406</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B3" t="n">
         <v>0.047</v>
@@ -866,12 +946,12 @@
         <v>105.559</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B4" t="n">
         <v>0.48</v>
@@ -879,12 +959,12 @@
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B5" t="n">
         <v>-36.508</v>
@@ -896,12 +976,12 @@
         <v>-54.79</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
         <v>0.019</v>
@@ -913,12 +993,12 @@
         <v>58.157</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B7" t="n">
         <v>0.185</v>
@@ -926,12 +1006,12 @@
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B8" t="n">
         <v>87.968</v>
@@ -943,12 +1023,12 @@
         <v>52.75</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B9" t="n">
         <v>-0.041</v>
@@ -960,12 +1040,12 @@
         <v>-49.84</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B10" t="n">
         <v>0.148</v>
@@ -973,7 +1053,7 @@
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -999,30 +1079,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C2" t="n">
         <v>7.6</v>
@@ -1039,10 +1119,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C3" t="n">
         <v>8.6</v>
@@ -1059,10 +1139,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C4" t="n">
         <v>6.9</v>
@@ -1079,10 +1159,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C5" t="n">
         <v>8.9</v>
@@ -1099,10 +1179,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C6" t="n">
         <v>7.3</v>
@@ -1119,10 +1199,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C7" t="n">
         <v>8.2</v>
@@ -1139,10 +1219,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C8" t="n">
         <v>7.5</v>
@@ -1159,10 +1239,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C9" t="n">
         <v>7.3</v>
@@ -1179,10 +1259,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C10" t="n">
         <v>7.1</v>
@@ -1199,10 +1279,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C11" t="n">
         <v>1.2</v>
@@ -1219,10 +1299,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C12" t="n">
         <v>1.6</v>
@@ -1239,10 +1319,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C13" t="n">
         <v>0.5</v>
@@ -1259,10 +1339,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
         <v>1.2</v>
@@ -1279,10 +1359,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C15" t="n">
         <v>1.2</v>
@@ -1299,10 +1379,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C16" t="n">
         <v>1.5</v>
@@ -1319,10 +1399,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -1339,10 +1419,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C18" t="n">
         <v>1.2</v>
@@ -1359,10 +1439,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C19" t="n">
         <v>1.6</v>
@@ -1379,10 +1459,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C20" t="n">
         <v>376.7</v>
@@ -1399,10 +1479,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C21" t="n">
         <v>304.6</v>
@@ -1419,10 +1499,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C22" t="n">
         <v>721.9</v>
@@ -1439,10 +1519,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C23" t="n">
         <v>334.2</v>
@@ -1459,10 +1539,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C24" t="n">
         <v>398.9</v>
@@ -1479,10 +1559,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C25" t="n">
         <v>364.9</v>
@@ -1499,10 +1579,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C26" t="n">
         <v>327.8</v>
@@ -1519,10 +1599,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C27" t="n">
         <v>449.2</v>
@@ -1539,10 +1619,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C28" t="n">
         <v>299.3</v>

</xml_diff>